<commit_message>
Added the updated version of Supplemental Table 7.
</commit_message>
<xml_diff>
--- a/Analysis/Genomics_manuscript_TIR/Supplemental_Figures/Supplemental_Table_7.xlsx
+++ b/Analysis/Genomics_manuscript_TIR/Supplemental_Figures/Supplemental_Table_7.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work_Files\GCMP_TIR\immunity_microbiome\Supplemental_Figures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BAD84AB-EE45-48FC-BB40-5E1D742DBA25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC2C811D-579C-4892-B9B0-9DC5D9FBA682}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3132" yWindow="1908" windowWidth="17280" windowHeight="8964" activeTab="3" xr2:uid="{1D9A66A8-7322-49B3-B858-11998F327895}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{1D9A66A8-7322-49B3-B858-11998F327895}"/>
   </bookViews>
   <sheets>
     <sheet name="Table S7A" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="32">
   <si>
     <t>Immune_Trait</t>
   </si>
@@ -113,28 +113,25 @@
     <t>lm(y_trait_positive ~ x_trait_positive -1)</t>
   </si>
   <si>
-    <t>Phylogenetic comparison of TIR, LRR, and Ig domains vs. Alpha Diversity in all compartments for all and unique isoforms.</t>
-  </si>
-  <si>
-    <t>Table S7A</t>
-  </si>
-  <si>
-    <t>Table S7B</t>
-  </si>
-  <si>
-    <t>Phylogenetic comparison of TIR, LRR, and Ig domains vs. Alpha Diversity in the mucus compartment for all and unique isoforms.</t>
-  </si>
-  <si>
-    <t>Table S7C</t>
-  </si>
-  <si>
-    <t>Phylogenetic comparison of TIR, LRR, and Ig domains vs. Alpha Diversity in the tissue compartment for all and unique isoforms.</t>
-  </si>
-  <si>
-    <t>Table S7D</t>
-  </si>
-  <si>
-    <t>Phylogenetic comparison of TIR, LRR, and Ig domains vs. Alpha Diversity in the skeleton compartment for all and unique isoforms.</t>
+    <t>Table S7D: Phylogenetic comparison of TIR, LRR, and Ig domains vs. Alpha Diversity in the skeleton compartment for all and unique isoforms</t>
+  </si>
+  <si>
+    <t>Table S7A: Phylogenetic comparison of TIR, LRR, and Ig domains vs Alpha Diversity in all compartments for all and unique isoforms</t>
+  </si>
+  <si>
+    <t>Table S7B: Phylogenic comarison of TIR, LRR, and Ig domains vs. Alpha Diversity in the mucus compatment for all and unique isoforms</t>
+  </si>
+  <si>
+    <t>Phylogenetic independent contranst results for TIR, LRR, and Ig domains for ln ASVs and Gini Index in the mucus compartment in the coral microbiome data collected during the Global Coral Microbiome Project. All analyses were conducted using the phyloseq package in R. Outputs were also corrected for multiple comparisons by domain analyzed (eg TIR total or TIR total unique).</t>
+  </si>
+  <si>
+    <t>Table S7C: Phylogenetic comparison of TIR, LRR, and Ig domains vs. Alpha Diversity in the tissue compartment for all and unique isoforms</t>
+  </si>
+  <si>
+    <t>Phylogenetic independent contranst results for TIR, LRR, and Ig domains for ln ASVs and Gini Index in all compartments combined in the coral microbiome data collected during the Global Coral Microbiome Project. All analyses were conducted using the phyloseq package in R. Outputs were also corrected for multiple comparisons by domain analyzed (eg TIR total or TIR total unique).</t>
+  </si>
+  <si>
+    <t>Phylogenetic independent contranst results for TIR, LRR, and Ig domains for ln ASVs and Gini Index in the skeletal compartment in the coral microbiome data collected during the Global Coral Microbiome Project. All analyses were conducted using the phyloseq package in R. Outputs were also corrected for multiple comparisons by domain analyzed (eg TIR total or TIR total unique).</t>
   </si>
 </sst>
 </file>
@@ -212,6 +209,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="11" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -219,9 +217,8 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="11" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -538,8 +535,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F45E0DC-CD8B-4D76-B79F-EC971B0A48B7}">
   <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -549,28 +546,39 @@
     <col min="3" max="3" width="13.5546875" style="1" customWidth="1"/>
     <col min="4" max="4" width="10.77734375" style="1" customWidth="1"/>
     <col min="5" max="5" width="34.44140625" style="1" customWidth="1"/>
-    <col min="6" max="7" width="8.88671875" style="1"/>
+    <col min="6" max="6" width="8.88671875" style="1"/>
+    <col min="7" max="7" width="13.33203125" style="1" customWidth="1"/>
     <col min="8" max="8" width="10.77734375" style="1" customWidth="1"/>
     <col min="9" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
     </row>
     <row r="2" spans="1:10" ht="28.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
+      <c r="A2" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -1054,8 +1062,8 @@
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1066,7 +1074,7 @@
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="A2" sqref="A2:J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1082,22 +1090,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-    </row>
-    <row r="2" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+    </row>
+    <row r="2" spans="1:10" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -1453,8 +1471,8 @@
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1465,7 +1483,7 @@
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1482,22 +1500,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-    </row>
-    <row r="2" spans="1:10" ht="19.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+    </row>
+    <row r="2" spans="1:10" ht="31.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -1853,8 +1881,8 @@
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1864,8 +1892,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F80615E1-7162-4E4A-9B78-187BC642500B}">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1882,22 +1910,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+    </row>
+    <row r="2" spans="1:10" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-    </row>
-    <row r="2" spans="1:10" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -2206,7 +2244,7 @@
       <c r="F12" s="3">
         <v>0.97842166399999997</v>
       </c>
-      <c r="G12" s="7">
+      <c r="G12" s="4">
         <v>8.5900000000000001E-5</v>
       </c>
       <c r="H12" s="3">
@@ -2253,8 +2291,8 @@
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>